<commit_message>
Update single_track_simulation.py and README.md
</commit_message>
<xml_diff>
--- a/input/layout.xlsx
+++ b/input/layout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qianqiantong/PycharmProjects/altrios-private/altrios/python/altrios/lifts/single_track_input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qianqiantong/PycharmProjects/LIFTS/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4F3668-89DD-1844-9784-0B1A8A5161B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013C57BD-F003-6C4B-9839-2B3644CA6FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A6382B0-CC3E-4A48-B9DD-BF4A5E344F0A}">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73:F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1861,6 +1861,26 @@
         <v>39</v>
       </c>
     </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>800</v>
+      </c>
+      <c r="B73" s="1">
+        <v>6</v>
+      </c>
+      <c r="C73" s="1">
+        <v>4</v>
+      </c>
+      <c r="D73" s="1">
+        <v>2</v>
+      </c>
+      <c r="E73" s="1">
+        <v>2</v>
+      </c>
+      <c r="F73" s="1">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>